<commit_message>
docs: add Equity Financing Strategies Guide with rate hierarchy, arb strategies, and DV01 risk management
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/data/Futures data B/Mid_Spreads_With_Formulas TESTING.xlsx
+++ b/data/Futures data B/Mid_Spreads_With_Formulas TESTING.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fdae8be99c1de88c/Desktop/Quarterback_v1/data/Futures data B/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{7CB1A42B-C0F1-44CC-B989-E36B3D80D5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63A04659-60A0-4196-9603-CE3D7C49F512}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{7CB1A42B-C0F1-44CC-B989-E36B3D80D5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{093317A8-3E19-45DF-A366-6CA895CB1492}"/>
   <bookViews>
-    <workbookView xWindow="16875" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mid Spreads" sheetId="1" r:id="rId1"/>
@@ -128,12 +128,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,10 +197,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -205,9 +214,11 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -513,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
@@ -690,39 +701,39 @@
       <c r="E6" s="3"/>
       <c r="F6" s="10">
         <f ca="1">(F4-($C$6*(($D$6-(TODAY()))/(F$5-(TODAY())))))/((F$2-$A$6)/F$2)</f>
-        <v>50.499999999999993</v>
+        <v>51.446808510638292</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" ref="F6:N6" ca="1" si="0">(G4-($C$6*(($D$6-(TODAY()))/(G$5-(TODAY())))))/((G$2-$A$6)/G$2)</f>
-        <v>132.7770083102493</v>
+        <v>133.36760233918127</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>110.8891108891109</v>
+        <v>111.29655207178143</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>80.527836390196398</v>
+        <v>80.749109643041621</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>56.291833785904686</v>
+        <v>56.444193080691932</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>83.52104737442923</v>
+        <v>83.637218784648965</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>67.462906292020222</v>
+        <v>67.556977905815117</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>69.892920588368284</v>
+        <v>69.971676562424165</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>75.953989588850234</v>
+        <v>76.021821718021258</v>
       </c>
       <c r="T6">
         <f>20*44.5</f>
@@ -746,35 +757,35 @@
       <c r="F7" s="3"/>
       <c r="G7" s="2">
         <f t="shared" ref="G7:N7" ca="1" si="1">(G4-($C$7*(($D$7-(TODAY()))/(G$5-(TODAY())))))/((G$2-$A$7)/G$2)</f>
-        <v>177.44736842105263</v>
+        <v>178.42</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>120.99325513196482</v>
+        <v>121.65981059485055</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>78.947344734473447</v>
+        <v>79.307327001356853</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>52.445733788395906</v>
+        <v>52.69315068493151</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>83.072916666666671</v>
+        <v>83.261395778938208</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>66.019269626195992</v>
+        <v>66.171810638318988</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>68.843424696781597</v>
+        <v>68.971083472853394</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>75.350968351440727</v>
+        <v>75.46089150546679</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.45">
@@ -795,31 +806,31 @@
       <c r="G8" s="3"/>
       <c r="H8" s="2">
         <f t="shared" ref="H8:N8" ca="1" si="2">(H4-($C$8*(($D$8-(TODAY()))/(H$5-(TODAY())))))/((H$2-$A$8)/H$2)</f>
-        <v>108.92245989304813</v>
+        <v>109.80194279546681</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>66.470297029702962</v>
+        <v>66.945273631840791</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>41.808103049653198</v>
+        <v>42.134555899248781</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>78.372395833333329</v>
+        <v>78.621083550913838</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>61.186602845450885</v>
+        <v>61.387872236446505</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>65.082130237253907</v>
+        <v>65.250568900126424</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>72.493994241807414</v>
+        <v>72.639031736702918</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.45">
@@ -841,27 +852,27 @@
       <c r="H9" s="3"/>
       <c r="I9" s="2">
         <f t="shared" ref="I9:N9" ca="1" si="3">(I4-($C$9*(($D$9-(TODAY()))/(I$5-(TODAY())))))/((I$2-$A$9)/I$2)</f>
-        <v>108.02125484287558</v>
+        <v>108.27874215877137</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>58.101997426285465</v>
+        <v>58.278969234224107</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>93.787399254866173</v>
+        <v>93.922214175449284</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>71.182825613205367</v>
+        <v>71.29193480937667</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>73.350857820345922</v>
+        <v>73.442169306008395</v>
       </c>
       <c r="N9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>79.84712517982409</v>
+        <v>79.925750769162164</v>
       </c>
       <c r="T9">
         <f>2352-934.5</f>
@@ -888,23 +899,23 @@
       <c r="I10" s="3"/>
       <c r="J10" s="2">
         <f ca="1">(J4-($C$10*(($D$10-(TODAY()))/(J$5-(TODAY())))))/((J$2-$A$10)/J$2)</f>
-        <v>57.916776056707782</v>
+        <v>58.104056902002121</v>
       </c>
       <c r="K10" s="2">
         <f ca="1">(K4-($C$10*(($D$10-(TODAY()))/(K$5-(TODAY())))))/((K$2-$A$10)/K$2)</f>
-        <v>111.75731169871796</v>
+        <v>111.89997991564572</v>
       </c>
       <c r="L10" s="2">
         <f ca="1">(L4-($C$10*(($D$10-(TODAY()))/(L$5-(TODAY())))))/((L$2-$A$10)/L$2)</f>
-        <v>75.570861255894769</v>
+        <v>75.686326327571209</v>
       </c>
       <c r="M10" s="2">
         <f ca="1">(M4-($C$10*(($D$10-(TODAY()))/(M$5-(TODAY())))))/((M$2-$A$10)/M$2)</f>
-        <v>77.182828214188646</v>
+        <v>77.279458815520755</v>
       </c>
       <c r="N10" s="2">
         <f ca="1">(N4-($C$10*(($D$10-(TODAY()))/(N$5-(TODAY())))))/((N$2-$A$10)/N$2)</f>
-        <v>84.229106661983366</v>
+        <v>84.312312382739194</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.45">
@@ -928,19 +939,19 @@
       <c r="J11" s="3"/>
       <c r="K11" s="2">
         <f ca="1">(K4-($C$11*(($D$11-(TODAY()))/(K$5-(TODAY())))))/((K$2-$A$11)/K$2)</f>
-        <v>164.0304487179487</v>
+        <v>164.1770435830488</v>
       </c>
       <c r="L11" s="2">
         <f ca="1">(L4-($C$11*(($D$11-(TODAY()))/(L$5-(TODAY())))))/((L$2-$A$11)/L$2)</f>
-        <v>83.673392078700147</v>
+        <v>83.79203508812914</v>
       </c>
       <c r="M11" s="2">
         <f ca="1">(M4-($C$11*(($D$11-(TODAY()))/(M$5-(TODAY())))))/((M$2-$A$11)/M$2)</f>
-        <v>83.098939929328623</v>
+        <v>83.198230088495578</v>
       </c>
       <c r="N11" s="2">
         <f ca="1">(N4-($C$11*(($D$11-(TODAY()))/(N$5-(TODAY())))))/((N$2-$A$11)/N$2)</f>
-        <v>90.431389767006209</v>
+        <v>90.516885553470928</v>
       </c>
       <c r="T11">
         <f>T9/28</f>
@@ -969,15 +980,15 @@
       <c r="K12" s="5"/>
       <c r="L12" s="2">
         <f ca="1">(L4-($C$12*(($D$12-(TODAY()))/(L$5-(TODAY())))))/((L$2-$A$12)/L$2)</f>
-        <v>19.60794655414908</v>
+        <v>19.772140004698176</v>
       </c>
       <c r="M12" s="2">
         <f ca="1">(M4-($C$12*(($D$12-(TODAY()))/(M$5-(TODAY())))))/((M$2-$A$12)/M$2)</f>
-        <v>51.156156564283762</v>
+        <v>51.293567052416613</v>
       </c>
       <c r="N12" s="2">
         <f ca="1">(N4-($C$12*(($D$12-(TODAY()))/(N$5-(TODAY())))))/((N$2-$A$12)/N$2)</f>
-        <v>71.592319400538585</v>
+        <v>71.710639462163854</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.45">
@@ -1003,11 +1014,11 @@
       <c r="L13" s="6"/>
       <c r="M13" s="2">
         <f ca="1">(M4-($C$13*(($D$13-(TODAY()))/(M$5-(TODAY())))))/((M$2-$A$13)/M$2)</f>
-        <v>82.025099861729956</v>
+        <v>82.143006925740693</v>
       </c>
       <c r="N13" s="2">
         <f ca="1">(N4-($C$13*(($D$13-(TODAY()))/(N$5-(TODAY())))))/((N$2-$A$13)/N$2)</f>
-        <v>97.164059186066822</v>
+        <v>97.265585432493651</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.45">
@@ -1034,7 +1045,7 @@
       <c r="M14" s="6"/>
       <c r="N14" s="2">
         <f ca="1">(N4-($C$14*(($D$14-(TODAY()))/(N$5-(TODAY())))))/((N$2-$A$14)/N$2)</f>
-        <v>112.48963821566561</v>
+        <v>112.5949812382739</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.45">
@@ -1350,10 +1361,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACDA5D3-FFEC-4ECE-89E0-6E66E569426D}">
-  <dimension ref="A2:N32"/>
+  <dimension ref="A2:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1363,9 +1374,10 @@
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="14" width="12" customWidth="1"/>
+    <col min="17" max="17" width="9.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="E2">
         <v>21</v>
       </c>
@@ -1397,7 +1409,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="D3" t="s">
         <v>0</v>
       </c>
@@ -1432,7 +1444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="E4">
         <v>44.5</v>
       </c>
@@ -1464,7 +1476,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1505,7 +1517,7 @@
         <v>46738</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>21</v>
       </c>
@@ -1521,42 +1533,45 @@
       <c r="E6" s="3"/>
       <c r="F6" s="2">
         <f t="shared" ref="F6:N6" ca="1" si="0">(F4-($C$6*(($D$6-(TODAY()))/(F$5-(TODAY())))))/((F$2-$A$6)/F$2)</f>
-        <v>93.552083333333329</v>
+        <v>94.518617021276597</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>114.52302631578947</v>
+        <v>115.12416666666665</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>53.537878787878782</v>
+        <v>53.949847094801221</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>55.874143183549123</v>
+        <v>56.096632223497899</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>57.036492517721186</v>
+        <v>57.18940990516333</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>79.519731570512832</v>
+        <v>79.636222132958437</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>67.611503001914528</v>
+        <v>67.705781821907223</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>70.020929600434897</v>
+        <v>70.099829816201506</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>76.073226621171827</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+        <v>76.141165237201832</v>
+      </c>
+      <c r="Q6">
+        <v>262000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>49</v>
       </c>
@@ -1573,38 +1588,41 @@
       <c r="F7" s="3"/>
       <c r="G7" s="2">
         <f t="shared" ref="G7:N7" ca="1" si="1">(G4-($C$7*(($D$7-(TODAY()))/(G$5-(TODAY())))))/((G$2-$A$7)/G$2)</f>
-        <v>136.19736842105263</v>
+        <v>137.16999999999999</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>35.952932551319648</v>
+        <v>36.619488014205388</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>49.28825382538254</v>
+        <v>49.648236092265947</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>53.045733788395907</v>
+        <v>53.293150684931504</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>78.489583333333343</v>
+        <v>78.67806244560488</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>66.019269626195992</v>
+        <v>66.171810638318988</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>68.843424696781597</v>
+        <v>68.971083472853394</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>75.350968351440727</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+        <v>75.46089150546679</v>
+      </c>
+      <c r="Q7">
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>77</v>
       </c>
@@ -1622,34 +1640,38 @@
       <c r="G8" s="3"/>
       <c r="H8" s="2">
         <f t="shared" ref="H8:N8" ca="1" si="2">(H4-($C$8*(($D$8-(TODAY()))/(H$5-(TODAY())))))/((H$2-$A$8)/H$2)</f>
-        <v>-46.151069518716596</v>
+        <v>-45.27158661629791</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>30.220297029702966</v>
+        <v>30.695273631840795</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>42.48552240449191</v>
+        <v>42.811975254087486</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>73.372395833333329</v>
+        <v>73.621083550913838</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>61.186602845450885</v>
+        <v>61.387872236446505</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>65.082130237253907</v>
+        <v>65.250568900126424</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>72.493994241807414</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+        <v>72.639031736702918</v>
+      </c>
+      <c r="Q8" s="12">
+        <f>Q6/Q7</f>
+        <v>2.6199999999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>111</v>
       </c>
@@ -1668,30 +1690,30 @@
       <c r="H9" s="3"/>
       <c r="I9" s="2">
         <f t="shared" ref="I9:N9" ca="1" si="3">(I4-($C$9*(($D$9-(TODAY()))/(I$5-(TODAY())))))/((I$2-$A$9)/I$2)</f>
-        <v>58.374515712440804</v>
+        <v>58.632003028336584</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>58.905276114810057</v>
+        <v>59.082247922748699</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>88.166961298661803</v>
+        <v>88.301776219244914</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>71.182825613205367</v>
+        <v>71.29193480937667</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>73.350857820345922</v>
+        <v>73.442169306008395</v>
       </c>
       <c r="N9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>79.84712517982409</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+        <v>79.925750769162164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>203</v>
       </c>
@@ -1711,26 +1733,26 @@
       <c r="I10" s="3"/>
       <c r="J10" s="2">
         <f ca="1">(J4-($C$10*(($D$10-(TODAY()))/(J$5-(TODAY())))))/((J$2-$A$10)/J$2)</f>
-        <v>59.532160672092402</v>
+        <v>59.719441517386734</v>
       </c>
       <c r="K10" s="2">
         <f ca="1">(K4-($C$10*(($D$10-(TODAY()))/(K$5-(TODAY())))))/((K$2-$A$10)/K$2)</f>
-        <v>103.2957732371795</v>
+        <v>103.43844145410726</v>
       </c>
       <c r="L10" s="2">
         <f ca="1">(L4-($C$10*(($D$10-(TODAY()))/(L$5-(TODAY())))))/((L$2-$A$10)/L$2)</f>
-        <v>75.570861255894769</v>
+        <v>75.686326327571209</v>
       </c>
       <c r="M10" s="2">
         <f ca="1">(M4-($C$10*(($D$10-(TODAY()))/(M$5-(TODAY())))))/((M$2-$A$10)/M$2)</f>
-        <v>77.182828214188646</v>
+        <v>77.279458815520755</v>
       </c>
       <c r="N10" s="2">
         <f ca="1">(N4-($C$10*(($D$10-(TODAY()))/(N$5-(TODAY())))))/((N$2-$A$10)/N$2)</f>
-        <v>84.229106661983366</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+        <v>84.312312382739194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>294</v>
       </c>
@@ -1751,22 +1773,22 @@
       <c r="J11" s="3"/>
       <c r="K11" s="2">
         <f ca="1">(K4-($C$11*(($D$11-(TODAY()))/(K$5-(TODAY())))))/((K$2-$A$11)/K$2)</f>
-        <v>147.10737179487177</v>
+        <v>147.25396665997187</v>
       </c>
       <c r="L11" s="2">
         <f ca="1">(L4-($C$11*(($D$11-(TODAY()))/(L$5-(TODAY())))))/((L$2-$A$11)/L$2)</f>
-        <v>83.673392078700147</v>
+        <v>83.79203508812914</v>
       </c>
       <c r="M11" s="2">
         <f ca="1">(M4-($C$11*(($D$11-(TODAY()))/(M$5-(TODAY())))))/((M$2-$A$11)/M$2)</f>
-        <v>83.098939929328623</v>
+        <v>83.198230088495578</v>
       </c>
       <c r="N11" s="2">
         <f ca="1">(N4-($C$11*(($D$11-(TODAY()))/(N$5-(TODAY())))))/((N$2-$A$11)/N$2)</f>
-        <v>90.431389767006209</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+        <v>90.516885553470928</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>385</v>
       </c>
@@ -1788,18 +1810,18 @@
       <c r="K12" s="5"/>
       <c r="L12" s="2">
         <f ca="1">(L4-($C$12*(($D$12-(TODAY()))/(L$5-(TODAY())))))/((L$2-$A$12)/L$2)</f>
-        <v>19.60794655414908</v>
+        <v>19.772140004698176</v>
       </c>
       <c r="M12" s="2">
         <f ca="1">(M4-($C$12*(($D$12-(TODAY()))/(M$5-(TODAY())))))/((M$2-$A$12)/M$2)</f>
-        <v>51.156156564283762</v>
+        <v>51.293567052416613</v>
       </c>
       <c r="N12" s="2">
         <f ca="1">(N4-($C$12*(($D$12-(TODAY()))/(N$5-(TODAY())))))/((N$2-$A$12)/N$2)</f>
-        <v>71.592319400538585</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+        <v>71.710639462163854</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>475</v>
       </c>
@@ -1822,14 +1844,14 @@
       <c r="L13" s="6"/>
       <c r="M13" s="2">
         <f ca="1">(M4-($C$13*(($D$13-(TODAY()))/(M$5-(TODAY())))))/((M$2-$A$13)/M$2)</f>
-        <v>82.025099861729956</v>
+        <v>82.143006925740693</v>
       </c>
       <c r="N13" s="2">
         <f ca="1">(N4-($C$13*(($D$13-(TODAY()))/(N$5-(TODAY())))))/((N$2-$A$13)/N$2)</f>
-        <v>97.164059186066822</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+        <v>97.265585432493651</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>567</v>
       </c>
@@ -1853,10 +1875,10 @@
       <c r="M14" s="6"/>
       <c r="N14" s="2">
         <f ca="1">(N4-($C$14*(($D$14-(TODAY()))/(N$5-(TODAY())))))/((N$2-$A$14)/N$2)</f>
-        <v>112.48963821566561</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+        <v>112.5949812382739</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>658</v>
       </c>
@@ -1880,7 +1902,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>749</v>
       </c>

</xml_diff>